<commit_message>
added movielens variation analysis
analysed how much % of authors used a variation of movielens (1m, 100k, ...)
</commit_message>
<xml_diff>
--- a/Popularity of Recommender System Datasets.xlsx
+++ b/Popularity of Recommender System Datasets.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Beel Group\Students\Victor Brunel, Intern Summer\Victor Brunel, TCD Summer Internship 2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE171CE-2181-4D5D-B83F-7F95CB1320AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A8F229-D38D-4AA4-BB56-F51A6EA99E41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="15034" xr2:uid="{0D86C001-5B52-4EBE-9AD0-E0858F57DF04}"/>
   </bookViews>
   <sheets>
     <sheet name="RecSyst all" sheetId="3" r:id="rId1"/>
+    <sheet name="MovieLens Popularity" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -706,7 +707,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="239">
   <si>
     <t>Paper Name (Title)</t>
   </si>
@@ -1381,13 +1382,55 @@
   </si>
   <si>
     <t>Total number of papers (incl. those not using offline datasets)</t>
+  </si>
+  <si>
+    <t>MovieLens Popularity</t>
+  </si>
+  <si>
+    <t>MovieLens 100k</t>
+  </si>
+  <si>
+    <t>MovieLens 1m</t>
+  </si>
+  <si>
+    <t>MovieLens Unkown</t>
+  </si>
+  <si>
+    <t>Total Manuscripts using MovieLens</t>
+  </si>
+  <si>
+    <t>MovieLens 2k</t>
+  </si>
+  <si>
+    <t>MovieLens 1M</t>
+  </si>
+  <si>
+    <t>MovieLens 10M</t>
+  </si>
+  <si>
+    <t>MovieLens 20M</t>
+  </si>
+  <si>
+    <t>MovieLens Latest, Full</t>
+  </si>
+  <si>
+    <t>MovieLens Latest, Small</t>
+  </si>
+  <si>
+    <t>MovieLens Variation</t>
+  </si>
+  <si>
+    <t>Relative Count</t>
+  </si>
+  <si>
+    <t>Absolute Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1476,6 +1519,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1536,7 +1585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1609,11 +1658,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2000,7 +2051,133 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1920" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Number of Datasets being used for Recommender-Systems Research </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1920" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>ACM RecSys 2017 &amp; 2018; Full- and Short Papers</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1920" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2198,7 +2375,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of datasets being used for research </a:t>
+                  <a:t>Number of datasets</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2281,7 +2458,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2356,33 +2533,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="1761964047"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -2447,7 +2597,1116 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Popularity of the different MovieLens Variations</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>ACM RecSys Conference 2017 &amp; 2018; Full- and Short Papers</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:pattFill prst="pct80">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RecSyst all'!$A$165:$A$173</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>MovieLens 2k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MovieLens 100k</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MovieLens 1M</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MovieLens 10M</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MovieLens 20M</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MovieLens Latest, Full</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MovieLens Latest, Small</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MovieLens  Tag Genome </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MovieLens Unkown</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RecSyst all'!$B$165:$B$173</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.8571428571428571E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42857142857142855</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11428571428571428</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8571428571428571E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11428571428571428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6D49-459F-AABE-53977BC97EDF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="267"/>
+        <c:overlap val="-43"/>
+        <c:axId val="1999386479"/>
+        <c:axId val="78910223"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1999386479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MovieLens Variation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-1920000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="78910223"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="78910223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distribution</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1999386479"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400">
+          <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Popularity of Recommender-Systems</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t> Datasets </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
+              <a:t>ACM RecSys 2017 &amp; 2018; Full- and Short Papers</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:pattFill prst="pct80">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'RecSyst all'!$A$144:$A$152</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>MovieLens</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Amazon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Yelp</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Proprietary</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Tripadvisor</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Yahoo!</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>BookCrossing</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Epinions</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>LastFM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'RecSyst all'!$B$144:$B$152</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.39772727272727271</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35227272727272729</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11363636363636363</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.9545454545454544E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6818181818181816E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.5454545454545456E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5454545454545456E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5454545454545456E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6CBA-41EF-A5BF-7341335C7998}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="267"/>
+        <c:overlap val="-43"/>
+        <c:axId val="1999386479"/>
+        <c:axId val="78910223"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1999386479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Dataset</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-1920000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="78910223"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="78910223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distribution</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1999386479"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400">
+          <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3036,20 +4295,1118 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="208">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="208">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>475340</xdr:colOff>
-      <xdr:row>142</xdr:row>
-      <xdr:rowOff>111579</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>306870</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>353787</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>81644</xdr:rowOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>101082</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>90717</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3203,6 +5560,78 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333995</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>15552</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>241041</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41968368-11DD-4705-8717-750A0C7A6899}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>414695</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>90715</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>20734</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40D106BA-BA1C-4FB9-AEAB-9D4985342D3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3689,11 +6118,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EA076A-3133-4A48-B225-9E4B426863E3}">
-  <dimension ref="A1:CH153"/>
+  <dimension ref="A1:CH175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K22" sqref="K22"/>
+      <selection pane="topRight" activeCell="AT145" sqref="AT145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -19067,16 +21496,16 @@
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
-      <c r="F125" s="32" t="s">
+      <c r="F125" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="G125" s="32"/>
-      <c r="H125" s="32"/>
-      <c r="I125" s="32"/>
-      <c r="J125" s="32"/>
-      <c r="K125" s="32"/>
-      <c r="L125" s="32"/>
-      <c r="M125" s="32"/>
+      <c r="G125" s="34"/>
+      <c r="H125" s="34"/>
+      <c r="I125" s="34"/>
+      <c r="J125" s="34"/>
+      <c r="K125" s="34"/>
+      <c r="L125" s="34"/>
+      <c r="M125" s="34"/>
     </row>
     <row r="126" spans="1:86" x14ac:dyDescent="0.4">
       <c r="A126" s="17" t="s">
@@ -19369,10 +21798,10 @@
       <c r="G143" s="3"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A144" s="33" t="s">
+      <c r="A144" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B144" s="34">
+      <c r="B144" s="33">
         <f>D122</f>
         <v>0.39772727272727271</v>
       </c>
@@ -19383,10 +21812,10 @@
       <c r="G144" s="3"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A145" s="33" t="s">
+      <c r="A145" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B145" s="34">
+      <c r="B145" s="33">
         <f>E122</f>
         <v>0.35227272727272729</v>
       </c>
@@ -19397,10 +21826,10 @@
       <c r="G145" s="3"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A146" s="33" t="s">
+      <c r="A146" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B146" s="34">
+      <c r="B146" s="33">
         <f>Q122</f>
         <v>0.125</v>
       </c>
@@ -19411,10 +21840,10 @@
       <c r="G146" s="3"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A147" s="33" t="s">
+      <c r="A147" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B147" s="34">
+      <c r="B147" s="33">
         <f>G122</f>
         <v>0.11363636363636363</v>
       </c>
@@ -19425,10 +21854,10 @@
       <c r="G147" s="3"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A148" s="33" t="s">
+      <c r="A148" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B148" s="34">
+      <c r="B148" s="33">
         <f>AE122</f>
         <v>7.9545454545454544E-2</v>
       </c>
@@ -19437,10 +21866,10 @@
       <c r="E148" s="3"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A149" s="33" t="s">
+      <c r="A149" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="B149" s="34">
+      <c r="B149" s="33">
         <f>F122</f>
         <v>5.6818181818181816E-2</v>
       </c>
@@ -19451,10 +21880,10 @@
       <c r="G149" s="3"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A150" s="33" t="s">
+      <c r="A150" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B150" s="34">
+      <c r="B150" s="33">
         <f>AB122</f>
         <v>4.5454545454545456E-2</v>
       </c>
@@ -19463,10 +21892,10 @@
       <c r="G150" s="3"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A151" s="33" t="s">
+      <c r="A151" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="B151" s="34">
+      <c r="B151" s="33">
         <f>BL122</f>
         <v>4.5454545454545456E-2</v>
       </c>
@@ -19477,10 +21906,10 @@
       <c r="G151" s="3"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A152" s="33" t="s">
+      <c r="A152" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="B152" s="34">
+      <c r="B152" s="33">
         <f>X122</f>
         <v>4.5454545454545456E-2</v>
       </c>
@@ -19496,6 +21925,151 @@
       <c r="E153" s="3"/>
       <c r="F153" s="3"/>
       <c r="G153" s="3"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A155" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A156" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A157" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A158" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A165" t="s">
+        <v>230</v>
+      </c>
+      <c r="B165" s="18">
+        <f>C165/$C$175</f>
+        <v>2.8571428571428571E-2</v>
+      </c>
+      <c r="C165">
+        <f>H116</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A166" t="s">
+        <v>226</v>
+      </c>
+      <c r="B166" s="18">
+        <f t="shared" ref="B166:B173" si="32">C166/$C$175</f>
+        <v>0.22857142857142856</v>
+      </c>
+      <c r="C166">
+        <f>I120</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A167" t="s">
+        <v>231</v>
+      </c>
+      <c r="B167" s="18">
+        <f t="shared" si="32"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="C167">
+        <f>L120</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A168" t="s">
+        <v>232</v>
+      </c>
+      <c r="B168" s="18">
+        <f t="shared" si="32"/>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="C168">
+        <f>K120</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A169" t="s">
+        <v>233</v>
+      </c>
+      <c r="B169" s="18">
+        <f t="shared" si="32"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="C169">
+        <f>J120</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A170" t="s">
+        <v>234</v>
+      </c>
+      <c r="B170" s="18">
+        <f t="shared" si="32"/>
+        <v>2.8571428571428571E-2</v>
+      </c>
+      <c r="C170">
+        <f>M120</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A171" t="s">
+        <v>235</v>
+      </c>
+      <c r="B171" s="18">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A172" t="s">
+        <v>30</v>
+      </c>
+      <c r="B172" s="18">
+        <f t="shared" si="32"/>
+        <v>8.5714285714285715E-2</v>
+      </c>
+      <c r="C172">
+        <f>N120</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A173" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B173" s="18">
+        <f t="shared" si="32"/>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="C173">
+        <f>O120</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A175" t="s">
+        <v>229</v>
+      </c>
+      <c r="C175">
+        <f>D120</f>
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -19530,4 +22104,161 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA5AB32-F9F6-4D07-82D3-FAC9110FCCCF}">
+  <dimension ref="A2:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="40.61328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.07421875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="35" t="str">
+        <f>'RecSyst all'!A165</f>
+        <v>MovieLens 2k</v>
+      </c>
+      <c r="B3" s="36">
+        <f>'RecSyst all'!B165</f>
+        <v>2.8571428571428571E-2</v>
+      </c>
+      <c r="C3" s="35">
+        <f>'RecSyst all'!C165</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="35" t="str">
+        <f>'RecSyst all'!A166</f>
+        <v>MovieLens 100k</v>
+      </c>
+      <c r="B4" s="36">
+        <f>'RecSyst all'!B166</f>
+        <v>0.22857142857142856</v>
+      </c>
+      <c r="C4" s="35">
+        <f>'RecSyst all'!C166</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="35" t="str">
+        <f>'RecSyst all'!A167</f>
+        <v>MovieLens 1M</v>
+      </c>
+      <c r="B5" s="36">
+        <f>'RecSyst all'!B167</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="C5" s="35">
+        <f>'RecSyst all'!C167</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="35" t="str">
+        <f>'RecSyst all'!A168</f>
+        <v>MovieLens 10M</v>
+      </c>
+      <c r="B6" s="36">
+        <f>'RecSyst all'!B168</f>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="C6" s="35">
+        <f>'RecSyst all'!C168</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="35" t="str">
+        <f>'RecSyst all'!A169</f>
+        <v>MovieLens 20M</v>
+      </c>
+      <c r="B7" s="36">
+        <f>'RecSyst all'!B169</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="C7" s="35">
+        <f>'RecSyst all'!C169</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="35" t="str">
+        <f>'RecSyst all'!A170</f>
+        <v>MovieLens Latest, Full</v>
+      </c>
+      <c r="B8" s="36">
+        <f>'RecSyst all'!B170</f>
+        <v>2.8571428571428571E-2</v>
+      </c>
+      <c r="C8" s="35">
+        <f>'RecSyst all'!C170</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="35" t="str">
+        <f>'RecSyst all'!A171</f>
+        <v>MovieLens Latest, Small</v>
+      </c>
+      <c r="B9" s="36">
+        <f>'RecSyst all'!B171</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="35">
+        <f>'RecSyst all'!C171</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="35" t="str">
+        <f>'RecSyst all'!A172</f>
+        <v xml:space="preserve">MovieLens  Tag Genome </v>
+      </c>
+      <c r="B10" s="36">
+        <f>'RecSyst all'!B172</f>
+        <v>8.5714285714285715E-2</v>
+      </c>
+      <c r="C10" s="35">
+        <f>'RecSyst all'!C172</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="35" t="str">
+        <f>'RecSyst all'!A173</f>
+        <v>MovieLens Unkown</v>
+      </c>
+      <c r="B11" s="36">
+        <f>'RecSyst all'!B173</f>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="C11" s="35">
+        <f>'RecSyst all'!C173</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>